<commit_message>
Deploy IG build aae93f80569cf0f971eb2a1e53fa0fd45e97066f
</commit_message>
<xml_diff>
--- a/currentbuild/StructureDefinition-no-basis-HumanName.xlsx
+++ b/currentbuild/StructureDefinition-no-basis-HumanName.xlsx
@@ -342,7 +342,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {http://hl7.no/fhir/ig/StructureDefinition/no-basis-middlename}
+    <t xml:space="preserve">Extension {http://hl7.no/fhir/StructureDefinition/no-basis-middlename}
 </t>
   </si>
   <si>
@@ -835,7 +835,7 @@
     <col min="8" max="8" width="13.953125" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="11.3671875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="58.91015625" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="56.9453125" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>

</xml_diff>